<commit_message>
Final data added with preliminary analysis
</commit_message>
<xml_diff>
--- a/Simulations/SRIM_ProtonsVsFilters/DataAnalysis/Rev2_Mixed/ThinFilter_Analysis.xlsx
+++ b/Simulations/SRIM_ProtonsVsFilters/DataAnalysis/Rev2_Mixed/ThinFilter_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Documents\GitHub\xmm-newton\Simulations\SRIM_ProtonsVsFilters\DataAnalysis\Rev2_Mixed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6750C0C2-D57E-4200-82C7-C33AC182F433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6921126-E9FE-455D-B1B2-7B07794EE3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A9EDBC4B-5209-4052-BD5C-CBCCBA64D68C}"/>
   </bookViews>
@@ -329,34 +329,34 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.3056097445</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.80427841249999998</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.9406773249</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.92068617019999999</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>1.053987142</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>0.96627441959999993</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>1.2317515479999999</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>1.01713531</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.77760495139999997</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>0.87851535430000005</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>1.1180000000000001</c:v>
@@ -392,34 +392,34 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.3056097445</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.80427841249999998</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.9406773249</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.92068617019999999</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>1.053987142</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>0.96627441959999993</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>1.2317515479999999</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>1.01713531</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.77760495139999997</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>0.87851535430000005</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>1.1180000000000001</c:v>
@@ -526,34 +526,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.63533932839999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.669453528</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12.53268008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>20.41206305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>28.94192649</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>38.011640620000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>47.403297030000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>57.116167619999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>67.708163709999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>77.806264809999988</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>98.4</c:v>
@@ -1008,34 +1008,34 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>4.5045716946000951</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>2.0329559294974144</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>1.3110612950010037</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.88351395978147196</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.76687841503915055</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>0.55895480572039868</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>0.58716430305214329</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>0.40751953276481645</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.25601406573579943</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>0.2505908384279274</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>0.2454146341463414</c:v>
@@ -1071,34 +1071,34 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>4.5045716946000951</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>2.0329559294974144</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>1.3110612950010037</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.88351395978147196</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.76687841503915055</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>0.55895480572039868</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>0.58716430305214329</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>0.40751953276481645</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.25601406573579943</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>0.2505908384279274</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>0.2454146341463414</c:v>
@@ -1205,34 +1205,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.3646606715999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>14.330546472</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>17.467319920000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>19.58793695</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>21.05807351</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>21.988359379999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>22.596702969999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>22.883832380000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>22.291836290000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>22.193735190000012</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>21.599999999999994</c:v>
@@ -1670,34 +1670,34 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.3056097445</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.80427841249999998</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.9406773249</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.92068617019999999</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>1.053987142</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.96627441959999993</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>1.2317515479999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>1.01713531</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>0.77760495139999997</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.87851535430000005</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>1.1180000000000001</c:v>
@@ -1730,34 +1730,34 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.3056097445</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.80427841249999998</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.9406773249</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.92068617019999999</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>1.053987142</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.96627441959999993</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>1.2317515479999999</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>1.01713531</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>0.77760495139999997</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.87851535430000005</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>1.1180000000000001</c:v>
@@ -1809,34 +1809,34 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>4.5045716946000951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>2.0329559294974144</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.3110612950010037</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.88351395978147196</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.76687841503915055</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.55895480572039868</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>0.58716430305214329</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>0.40751953276481645</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>0.25601406573579943</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.2505908384279274</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>0.2454146341463414</c:v>
@@ -1869,34 +1869,34 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>4.5045716946000951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>2.0329559294974144</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.3110612950010037</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.88351395978147196</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.76687841503915055</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.55895480572039868</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>0.58716430305214329</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>0.40751953276481645</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>0.25601406573579943</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>0.2505908384279274</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>0.2454146341463414</c:v>
@@ -1943,34 +1943,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.63533932839999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.669453528</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12.53268008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>20.41206305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>28.94192649</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>38.011640620000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>47.403297030000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>57.116167619999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>67.708163709999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>77.806264809999988</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>98.4</c:v>
@@ -2003,34 +2003,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.3646606715999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>14.330546472</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>17.467319920000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>19.58793695</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>21.05807351</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>21.988359379999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>22.596702969999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>22.883832380000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>22.291836290000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>22.193735190000012</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>21.599999999999994</c:v>
@@ -4437,7 +4437,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4535,12 +4535,16 @@
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
       <c r="C6" s="4">
         <f>B6/1000</f>
         <v>0</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
       <c r="E6" s="4">
         <f>D6/1000</f>
         <v>0</v>
@@ -4556,287 +4560,349 @@
         <f>F6*G6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>10</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <v>635.3393284</v>
+      </c>
       <c r="C7" s="4">
         <f t="shared" ref="C7:C23" si="0">B7/1000</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>0.63533932839999996</v>
+      </c>
+      <c r="D7" s="6">
+        <v>305.60974449999998</v>
+      </c>
       <c r="E7" s="4">
         <f t="shared" ref="E7:E23" si="1">D7/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="5" t="e">
+        <v>0.3056097445</v>
+      </c>
+      <c r="F7" s="5">
         <f>E7/C7</f>
-        <v>#DIV/0!</v>
+        <v>0.48101814391000958</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" ref="G7:G21" si="2">A7-C7</f>
-        <v>10</v>
-      </c>
-      <c r="H7" s="8" t="e">
+        <v>9.3646606715999994</v>
+      </c>
+      <c r="H7" s="8">
         <f t="shared" ref="H7:H21" si="3">F7*G7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>4.5045716946000951</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.36009999999999998</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>20</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="6">
+        <v>5669.453528</v>
+      </c>
       <c r="C8" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>5.669453528</v>
+      </c>
+      <c r="D8" s="6">
+        <v>804.27841249999994</v>
+      </c>
       <c r="E8" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="5" t="e">
+        <v>0.80427841249999998</v>
+      </c>
+      <c r="F8" s="5">
         <f t="shared" ref="F8:F21" si="4">E8/C8</f>
-        <v>#DIV/0!</v>
+        <v>0.14186171709987072</v>
       </c>
       <c r="G8" s="8">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="H8" s="8" t="e">
+        <v>14.330546472</v>
+      </c>
+      <c r="H8" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>2.0329559294974144</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.96860000000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>30</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <v>12532.68008</v>
+      </c>
       <c r="C9" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="6"/>
+        <v>12.53268008</v>
+      </c>
+      <c r="D9" s="6">
+        <v>940.67732490000003</v>
+      </c>
       <c r="E9" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5" t="e">
+        <v>0.9406773249</v>
+      </c>
+      <c r="F9" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>7.5057953996700122E-2</v>
       </c>
       <c r="G9" s="8">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="H9" s="8" t="e">
+        <v>17.467319920000001</v>
+      </c>
+      <c r="H9" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" s="7"/>
+        <v>1.3110612950010037</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.99370000000000003</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>40</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6">
+        <v>20412.063050000001</v>
+      </c>
       <c r="C10" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>20.41206305</v>
+      </c>
+      <c r="D10" s="6">
+        <v>920.68617019999999</v>
+      </c>
       <c r="E10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="5" t="e">
+        <v>0.92068617019999999</v>
+      </c>
+      <c r="F10" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>4.5105003249536799E-2</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="H10" s="8" t="e">
+        <v>19.58793695</v>
+      </c>
+      <c r="H10" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" s="7"/>
+        <v>0.88351395978147196</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.99629999999999996</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>50</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6">
+        <v>28941.926490000002</v>
+      </c>
       <c r="C11" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="6"/>
+        <v>28.94192649</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1053.9871419999999</v>
+      </c>
       <c r="E11" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="5" t="e">
+        <v>1.053987142</v>
+      </c>
+      <c r="F11" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>3.6417311140783011E-2</v>
       </c>
       <c r="G11" s="8">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="H11" s="8" t="e">
+        <v>21.05807351</v>
+      </c>
+      <c r="H11" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>0.76687841503915055</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.99870000000000003</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>60</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6">
+        <v>38011.640619999998</v>
+      </c>
       <c r="C12" s="8">
         <f>B12/1000</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="6"/>
+        <v>38.011640620000001</v>
+      </c>
+      <c r="D12" s="6">
+        <v>966.27441959999999</v>
+      </c>
       <c r="E12" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="5" t="e">
+        <v>0.96627441959999993</v>
+      </c>
+      <c r="F12" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2.542048708867331E-2</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="H12" s="8" t="e">
+        <v>21.988359379999999</v>
+      </c>
+      <c r="H12" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" s="7"/>
+        <v>0.55895480572039868</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.99890000000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>70</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6">
+        <v>47403.297030000002</v>
+      </c>
       <c r="C13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>47.403297030000004</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1231.751548</v>
+      </c>
       <c r="E13" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="5" t="e">
+        <v>1.2317515479999999</v>
+      </c>
+      <c r="F13" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2.598451215788776E-2</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="H13" s="8" t="e">
+        <v>22.596702969999996</v>
+      </c>
+      <c r="H13" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" s="7"/>
+        <v>0.58716430305214329</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.99970000000000003</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>80</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="6">
+        <v>57116.16762</v>
+      </c>
       <c r="C14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="6"/>
+        <v>57.116167619999999</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1017.13531</v>
+      </c>
       <c r="E14" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="5" t="e">
+        <v>1.01713531</v>
+      </c>
+      <c r="F14" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.7808185534560206E-2</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="H14" s="8" t="e">
+        <v>22.883832380000001</v>
+      </c>
+      <c r="H14" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" s="7"/>
+        <v>0.40751953276481645</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0.99980000000000002</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>90</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6">
+        <v>67708.163709999993</v>
+      </c>
       <c r="C15" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="6"/>
+        <v>67.708163709999994</v>
+      </c>
+      <c r="D15" s="6">
+        <v>777.6049514</v>
+      </c>
       <c r="E15" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="5" t="e">
+        <v>0.77760495139999997</v>
+      </c>
+      <c r="F15" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.1484655745953327E-2</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="H15" s="8" t="e">
+        <v>22.291836290000006</v>
+      </c>
+      <c r="H15" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="7"/>
+        <v>0.25601406573579943</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.99990000000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>100</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6">
+        <v>77806.264809999993</v>
+      </c>
       <c r="C16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D16" s="6"/>
+        <v>77.806264809999988</v>
+      </c>
+      <c r="D16" s="6">
+        <v>878.51535430000001</v>
+      </c>
       <c r="E16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="5" t="e">
+        <v>0.87851535430000005</v>
+      </c>
+      <c r="F16" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.1291061927279274E-2</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="H16" s="8" t="e">
+        <v>22.193735190000012</v>
+      </c>
+      <c r="H16" s="8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="7"/>
+        <v>0.2505908384279274</v>
+      </c>
+      <c r="I16" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
@@ -4868,7 +4934,9 @@
         <f t="shared" si="3"/>
         <v>0.2454146341463414</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
@@ -4900,7 +4968,9 @@
         <f t="shared" si="3"/>
         <v>0.16626803086212683</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
@@ -4932,7 +5002,9 @@
         <f t="shared" si="3"/>
         <v>0.11291633977605016</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
@@ -4964,7 +5036,9 @@
         <f t="shared" si="3"/>
         <v>7.5285182427401356E-2</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
@@ -4996,7 +5070,9 @@
         <f t="shared" si="3"/>
         <v>5.9393100417490692E-2</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
@@ -5029,7 +5105,9 @@
         <f t="shared" ref="H22:H23" si="6">F22*G22</f>
         <v>4.8170140230515981E-2</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -5062,7 +5140,9 @@
         <f t="shared" si="6"/>
         <v>3.8659206816780943E-2</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="7">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>